<commit_message>
Made all the routes authorized acc. to profiles
</commit_message>
<xml_diff>
--- a/downloads/leads.xlsx
+++ b/downloads/leads.xlsx
@@ -32,9 +32,8 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:vt="http://schemas.openxmlformats.org/officeDocument/2006/docPropsVTypes">
-  <numFmts count="2">
+  <numFmts count="1">
     <numFmt numFmtId="56" formatCode="&quot;上午/下午 &quot;hh&quot;時&quot;mm&quot;分&quot;ss&quot;秒 &quot;"/>
-    <numFmt numFmtId="164" formatCode="[$-14009]yyyy/mm/dd;@"/>
   </numFmts>
   <fonts count="1">
     <font>
@@ -398,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:DA7"/>
+  <dimension ref="A1:DY3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -719,6 +718,78 @@
       <c r="DA1" t="str">
         <v>__v</v>
       </c>
+      <c r="DB1" t="str">
+        <v>assignBy_buffer_0</v>
+      </c>
+      <c r="DC1" t="str">
+        <v>assignBy_buffer_1</v>
+      </c>
+      <c r="DD1" t="str">
+        <v>assignBy_buffer_2</v>
+      </c>
+      <c r="DE1" t="str">
+        <v>assignBy_buffer_3</v>
+      </c>
+      <c r="DF1" t="str">
+        <v>assignBy_buffer_4</v>
+      </c>
+      <c r="DG1" t="str">
+        <v>assignBy_buffer_5</v>
+      </c>
+      <c r="DH1" t="str">
+        <v>assignBy_buffer_6</v>
+      </c>
+      <c r="DI1" t="str">
+        <v>assignBy_buffer_7</v>
+      </c>
+      <c r="DJ1" t="str">
+        <v>assignBy_buffer_8</v>
+      </c>
+      <c r="DK1" t="str">
+        <v>assignBy_buffer_9</v>
+      </c>
+      <c r="DL1" t="str">
+        <v>assignBy_buffer_10</v>
+      </c>
+      <c r="DM1" t="str">
+        <v>assignBy_buffer_11</v>
+      </c>
+      <c r="DN1" t="str">
+        <v>assignTo_buffer_0</v>
+      </c>
+      <c r="DO1" t="str">
+        <v>assignTo_buffer_1</v>
+      </c>
+      <c r="DP1" t="str">
+        <v>assignTo_buffer_2</v>
+      </c>
+      <c r="DQ1" t="str">
+        <v>assignTo_buffer_3</v>
+      </c>
+      <c r="DR1" t="str">
+        <v>assignTo_buffer_4</v>
+      </c>
+      <c r="DS1" t="str">
+        <v>assignTo_buffer_5</v>
+      </c>
+      <c r="DT1" t="str">
+        <v>assignTo_buffer_6</v>
+      </c>
+      <c r="DU1" t="str">
+        <v>assignTo_buffer_7</v>
+      </c>
+      <c r="DV1" t="str">
+        <v>assignTo_buffer_8</v>
+      </c>
+      <c r="DW1" t="str">
+        <v>assignTo_buffer_9</v>
+      </c>
+      <c r="DX1" t="str">
+        <v>assignTo_buffer_10</v>
+      </c>
+      <c r="DY1" t="str">
+        <v>assignTo_buffer_11</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
@@ -1036,527 +1107,132 @@
       <c r="DA2">
         <v>0</v>
       </c>
+      <c r="DB2">
+        <v>102</v>
+      </c>
+      <c r="DC2">
+        <v>152</v>
+      </c>
+      <c r="DD2">
+        <v>189</v>
+      </c>
+      <c r="DE2">
+        <v>80</v>
+      </c>
+      <c r="DF2">
+        <v>73</v>
+      </c>
+      <c r="DG2">
+        <v>9</v>
+      </c>
+      <c r="DH2">
+        <v>68</v>
+      </c>
+      <c r="DI2">
+        <v>85</v>
+      </c>
+      <c r="DJ2">
+        <v>53</v>
+      </c>
+      <c r="DK2">
+        <v>250</v>
+      </c>
+      <c r="DL2">
+        <v>106</v>
+      </c>
+      <c r="DM2">
+        <v>109</v>
+      </c>
+      <c r="DN2">
+        <v>102</v>
+      </c>
+      <c r="DO2">
+        <v>152</v>
+      </c>
+      <c r="DP2">
+        <v>192</v>
+      </c>
+      <c r="DQ2">
+        <v>219</v>
+      </c>
+      <c r="DR2">
+        <v>167</v>
+      </c>
+      <c r="DS2">
+        <v>9</v>
+      </c>
+      <c r="DT2">
+        <v>148</v>
+      </c>
+      <c r="DU2">
+        <v>134</v>
+      </c>
+      <c r="DV2">
+        <v>129</v>
+      </c>
+      <c r="DW2">
+        <v>46</v>
+      </c>
+      <c r="DX2">
+        <v>74</v>
+      </c>
+      <c r="DY2">
+        <v>19</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>Ram kumar</v>
+        <v>Hitesh</v>
       </c>
       <c r="B3" t="str">
-        <v>RMK@example.com</v>
+        <v>hitesh@example.com</v>
       </c>
       <c r="C3" t="str">
-        <v>123-456-7890</v>
+        <v>9898989901</v>
       </c>
       <c r="D3" t="str">
-        <v>Paris</v>
+        <v>Mumbai</v>
       </c>
       <c r="E3">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="F3">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="G3" t="b">
         <v>1</v>
       </c>
       <c r="H3" t="str">
-        <v>5-star</v>
+        <v>8 Start</v>
       </c>
       <c r="I3" t="str">
-        <v>123 Main St</v>
+        <v>Saket, New Delhi</v>
       </c>
       <c r="J3" t="str">
-        <v>New York</v>
+        <v>Delhi</v>
       </c>
       <c r="K3" t="str">
-        <v>10 days</v>
+        <v>5 days</v>
       </c>
       <c r="L3" t="str">
-        <v>2000 USD</v>
+        <v>20003</v>
       </c>
       <c r="M3" t="str">
-        <v>Car</v>
-      </c>
-      <c r="N3" t="str">
-        <v>Required</v>
+        <v>flight</v>
       </c>
       <c r="O3" t="str">
-        <v>New</v>
-      </c>
-      <c r="P3" t="str">
-        <v>Delta</v>
-      </c>
-      <c r="Q3" t="str">
-        <v>Expedia</v>
-      </c>
-      <c r="R3" t="str">
-        <v>Economy</v>
-      </c>
-      <c r="S3" t="str">
-        <v>Confirmed</v>
-      </c>
-      <c r="T3" t="str">
-        <v>USA</v>
-      </c>
-      <c r="U3" t="str">
-        <v>ABC123</v>
-      </c>
-      <c r="V3">
-        <v>2</v>
-      </c>
-      <c r="W3" t="str">
-        <v>Delta</v>
-      </c>
-      <c r="X3" t="str">
-        <v>Expedia</v>
-      </c>
-      <c r="Y3" t="str">
-        <v>Economy</v>
-      </c>
-      <c r="Z3" t="str">
-        <v>USA</v>
-      </c>
-      <c r="AA3" t="str">
-        <v>Confirmed</v>
-      </c>
-      <c r="AB3" t="str">
-        <v>XYZ456</v>
-      </c>
-      <c r="AC3">
-        <v>2</v>
-      </c>
-      <c r="AD3">
-        <v>500</v>
-      </c>
-      <c r="AE3">
-        <v>450</v>
-      </c>
-      <c r="AF3" t="str">
-        <v>Hilton</v>
-      </c>
-      <c r="AG3" t="str">
-        <v>Luxury</v>
-      </c>
-      <c r="AH3" t="str">
-        <v>Paris</v>
-      </c>
-      <c r="AI3">
-        <v>2</v>
-      </c>
-      <c r="AJ3" t="str">
-        <v>France</v>
-      </c>
-      <c r="AK3" t="str">
-        <v>Suite</v>
-      </c>
-      <c r="AL3">
-        <v>1500</v>
-      </c>
-      <c r="AM3">
-        <v>1400</v>
-      </c>
-      <c r="AN3" t="str">
-        <v>JFK</v>
-      </c>
-      <c r="AO3" t="str">
-        <v>2024-08-01T06:00:00.000Z</v>
-      </c>
-      <c r="AP3" t="str">
-        <v>Hilton</v>
-      </c>
-      <c r="AQ3" t="str">
-        <v>2024-08-01T08:00:00.000Z</v>
-      </c>
-      <c r="AR3" t="str">
-        <v>CDG</v>
-      </c>
-      <c r="AS3" t="str">
-        <v>2024-08-10T14:00:00.000Z</v>
-      </c>
-      <c r="AT3" t="str">
-        <v>2024-08-10T16:00:00.000Z</v>
-      </c>
-      <c r="AU3" t="str">
-        <v>Hilton</v>
-      </c>
-      <c r="AV3" t="str">
-        <v>Schengen Visa</v>
-      </c>
-      <c r="AW3" t="str">
-        <v>X1234567</v>
-      </c>
-      <c r="AX3" t="str">
-        <v>123456789</v>
-      </c>
-      <c r="AY3" t="str">
-        <v>Allianz</v>
-      </c>
-      <c r="AZ3" t="str">
-        <v>AX123456789</v>
-      </c>
-      <c r="BA3" t="str">
-        <v>flights</v>
-      </c>
-      <c r="BB3" t="str">
-        <v>Delta</v>
-      </c>
-      <c r="BC3" t="str">
-        <v>Expedia</v>
-      </c>
-      <c r="BD3" t="str">
-        <v>2024-08-01T10:00:00.000Z</v>
-      </c>
-      <c r="BE3" t="str">
-        <v>Economy</v>
-      </c>
-      <c r="BF3" t="str">
-        <v>Confirmed</v>
-      </c>
-      <c r="BG3" t="str">
-        <v>2024-08-01T08:00:00.000Z</v>
-      </c>
-      <c r="BH3" t="str">
-        <v>2024-08-01T12:00:00.000Z</v>
-      </c>
-      <c r="BI3" t="str">
-        <v>USA</v>
-      </c>
-      <c r="BJ3" t="str">
-        <v>ABC123</v>
-      </c>
-      <c r="BK3">
-        <v>2</v>
-      </c>
-      <c r="BL3" t="str">
-        <v>Delta</v>
-      </c>
-      <c r="BM3" t="str">
-        <v>Expedia</v>
-      </c>
-      <c r="BN3" t="str">
-        <v>2024-08-10T18:00:00.000Z</v>
-      </c>
-      <c r="BO3" t="str">
-        <v>Economy</v>
-      </c>
-      <c r="BP3" t="str">
-        <v>USA</v>
-      </c>
-      <c r="BQ3" t="str">
-        <v>Confirmed</v>
-      </c>
-      <c r="BR3" t="str">
-        <v>2024-08-10T16:00:00.000Z</v>
-      </c>
-      <c r="BS3" t="str">
-        <v>2024-08-10T20:00:00.000Z</v>
-      </c>
-      <c r="BT3" t="str">
-        <v>XYZ456</v>
-      </c>
-      <c r="BU3">
-        <v>2</v>
-      </c>
-      <c r="BV3">
-        <v>500</v>
-      </c>
-      <c r="BW3">
-        <v>450</v>
-      </c>
-      <c r="BX3" t="str">
-        <v>hotels</v>
-      </c>
-      <c r="BY3" t="str">
-        <v>Hilton</v>
-      </c>
-      <c r="BZ3" t="str">
-        <v>2024-08-01T15:00:00.000Z</v>
-      </c>
-      <c r="CA3" t="str">
-        <v>Luxury</v>
-      </c>
-      <c r="CB3" t="str">
-        <v>2024-08-01T15:00:00.000Z</v>
-      </c>
-      <c r="CC3" t="str">
-        <v>2024-08-10T11:00:00.000Z</v>
-      </c>
-      <c r="CD3" t="str">
-        <v>Paris</v>
-      </c>
-      <c r="CE3">
-        <v>2</v>
-      </c>
-      <c r="CF3" t="str">
-        <v>France</v>
-      </c>
-      <c r="CG3" t="str">
-        <v>Suite</v>
-      </c>
-      <c r="CH3">
-        <v>1500</v>
-      </c>
-      <c r="CI3">
-        <v>1400</v>
-      </c>
-      <c r="CJ3" t="str">
-        <v>transfers</v>
-      </c>
-      <c r="CK3" t="str">
-        <v>JFK</v>
-      </c>
-      <c r="CL3" t="str">
-        <v>2024-08-01T06:00:00.000Z</v>
-      </c>
-      <c r="CM3" t="str">
-        <v>Hilton</v>
-      </c>
-      <c r="CN3" t="str">
-        <v>2024-08-01T08:00:00.000Z</v>
-      </c>
-      <c r="CO3" t="str">
-        <v>CDG</v>
-      </c>
-      <c r="CP3" t="str">
-        <v>2024-08-10T14:00:00.000Z</v>
-      </c>
-      <c r="CQ3" t="str">
-        <v>2024-08-10T16:00:00.000Z</v>
-      </c>
-      <c r="CR3" t="str">
-        <v>Hilton</v>
-      </c>
-      <c r="CS3" t="str">
-        <v>visas</v>
-      </c>
-      <c r="CT3" t="str">
-        <v>Schengen Visa</v>
-      </c>
-      <c r="CU3" t="str">
-        <v>X1234567</v>
-      </c>
-      <c r="CV3" t="str">
-        <v>123456789</v>
-      </c>
-      <c r="CW3" t="str">
-        <v>insurances</v>
-      </c>
-      <c r="CX3" t="str">
-        <v>Allianz</v>
-      </c>
-      <c r="CY3" t="str">
-        <v>AX123456789</v>
+        <v>New lead</v>
       </c>
       <c r="CZ3">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="DA3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="str">
-        <v>Aditya</v>
-      </c>
-      <c r="B4" t="str">
-        <v>adi@adi.com</v>
-      </c>
-      <c r="C4" t="str">
-        <v>9898989898</v>
-      </c>
-      <c r="D4" t="str">
-        <v>Mumbai</v>
-      </c>
-      <c r="E4">
-        <v>8</v>
-      </c>
-      <c r="F4">
-        <v>22</v>
-      </c>
-      <c r="G4" t="b">
-        <v>1</v>
-      </c>
-      <c r="H4" t="str">
-        <v>5 Start</v>
-      </c>
-      <c r="I4" t="str">
-        <v>Saket, New Delhi</v>
-      </c>
-      <c r="J4" t="str">
-        <v>Delhi</v>
-      </c>
-      <c r="K4" t="str">
-        <v>2 days</v>
-      </c>
-      <c r="L4" t="str">
-        <v>20000</v>
-      </c>
-      <c r="M4" t="str">
-        <v>flight</v>
-      </c>
-      <c r="O4" t="str">
-        <v>New lead</v>
-      </c>
-      <c r="CZ4">
-        <v>45</v>
-      </c>
-      <c r="DA4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="str">
-        <v>Palak</v>
-      </c>
-      <c r="B5" t="str">
-        <v>palak@example.com</v>
-      </c>
-      <c r="C5" t="str">
-        <v>9898989899</v>
-      </c>
-      <c r="D5" t="str">
-        <v>Mumbai</v>
-      </c>
-      <c r="E5">
-        <v>8</v>
-      </c>
-      <c r="F5">
-        <v>22</v>
-      </c>
-      <c r="G5" t="b">
-        <v>1</v>
-      </c>
-      <c r="H5" t="str">
-        <v>6 Start</v>
-      </c>
-      <c r="I5" t="str">
-        <v>Saket, New Delhi</v>
-      </c>
-      <c r="J5" t="str">
-        <v>Delhi</v>
-      </c>
-      <c r="K5" t="str">
-        <v>3 days</v>
-      </c>
-      <c r="L5" t="str">
-        <v>20001</v>
-      </c>
-      <c r="M5" t="str">
-        <v>flight</v>
-      </c>
-      <c r="O5" t="str">
-        <v>New lead</v>
-      </c>
-      <c r="CZ5">
-        <v>46</v>
-      </c>
-      <c r="DA5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="str">
-        <v>Tarun</v>
-      </c>
-      <c r="B6" t="str">
-        <v>tarun@example.com</v>
-      </c>
-      <c r="C6" t="str">
-        <v>9898989900</v>
-      </c>
-      <c r="D6" t="str">
-        <v>Mumbai</v>
-      </c>
-      <c r="E6">
-        <v>8</v>
-      </c>
-      <c r="F6">
-        <v>22</v>
-      </c>
-      <c r="G6" t="b">
-        <v>1</v>
-      </c>
-      <c r="H6" t="str">
-        <v>7 Start</v>
-      </c>
-      <c r="I6" t="str">
-        <v>Saket, New Delhi</v>
-      </c>
-      <c r="J6" t="str">
-        <v>Delhi</v>
-      </c>
-      <c r="K6" t="str">
-        <v>4 days</v>
-      </c>
-      <c r="L6" t="str">
-        <v>20002</v>
-      </c>
-      <c r="M6" t="str">
-        <v>flight</v>
-      </c>
-      <c r="O6" t="str">
-        <v>New lead</v>
-      </c>
-      <c r="CZ6">
-        <v>47</v>
-      </c>
-      <c r="DA6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="str">
-        <v>Hitesh</v>
-      </c>
-      <c r="B7" t="str">
-        <v>hitesh@example.com</v>
-      </c>
-      <c r="C7" t="str">
-        <v>9898989901</v>
-      </c>
-      <c r="D7" t="str">
-        <v>Mumbai</v>
-      </c>
-      <c r="E7">
-        <v>8</v>
-      </c>
-      <c r="F7">
-        <v>22</v>
-      </c>
-      <c r="G7" t="b">
-        <v>1</v>
-      </c>
-      <c r="H7" t="str">
-        <v>8 Start</v>
-      </c>
-      <c r="I7" t="str">
-        <v>Saket, New Delhi</v>
-      </c>
-      <c r="J7" t="str">
-        <v>Delhi</v>
-      </c>
-      <c r="K7" t="str">
-        <v>5 days</v>
-      </c>
-      <c r="L7" t="str">
-        <v>20003</v>
-      </c>
-      <c r="M7" t="str">
-        <v>flight</v>
-      </c>
-      <c r="O7" t="str">
-        <v>New lead</v>
-      </c>
-      <c r="CZ7">
-        <v>48</v>
-      </c>
-      <c r="DA7">
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:DA7"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:DY3"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Pagination and Personalised Todos
</commit_message>
<xml_diff>
--- a/downloads/leads.xlsx
+++ b/downloads/leads.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:DY3"/>
+  <dimension ref="A1:DA3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -718,78 +718,6 @@
       <c r="DA1" t="str">
         <v>__v</v>
       </c>
-      <c r="DB1" t="str">
-        <v>assignBy_buffer_0</v>
-      </c>
-      <c r="DC1" t="str">
-        <v>assignBy_buffer_1</v>
-      </c>
-      <c r="DD1" t="str">
-        <v>assignBy_buffer_2</v>
-      </c>
-      <c r="DE1" t="str">
-        <v>assignBy_buffer_3</v>
-      </c>
-      <c r="DF1" t="str">
-        <v>assignBy_buffer_4</v>
-      </c>
-      <c r="DG1" t="str">
-        <v>assignBy_buffer_5</v>
-      </c>
-      <c r="DH1" t="str">
-        <v>assignBy_buffer_6</v>
-      </c>
-      <c r="DI1" t="str">
-        <v>assignBy_buffer_7</v>
-      </c>
-      <c r="DJ1" t="str">
-        <v>assignBy_buffer_8</v>
-      </c>
-      <c r="DK1" t="str">
-        <v>assignBy_buffer_9</v>
-      </c>
-      <c r="DL1" t="str">
-        <v>assignBy_buffer_10</v>
-      </c>
-      <c r="DM1" t="str">
-        <v>assignBy_buffer_11</v>
-      </c>
-      <c r="DN1" t="str">
-        <v>assignTo_buffer_0</v>
-      </c>
-      <c r="DO1" t="str">
-        <v>assignTo_buffer_1</v>
-      </c>
-      <c r="DP1" t="str">
-        <v>assignTo_buffer_2</v>
-      </c>
-      <c r="DQ1" t="str">
-        <v>assignTo_buffer_3</v>
-      </c>
-      <c r="DR1" t="str">
-        <v>assignTo_buffer_4</v>
-      </c>
-      <c r="DS1" t="str">
-        <v>assignTo_buffer_5</v>
-      </c>
-      <c r="DT1" t="str">
-        <v>assignTo_buffer_6</v>
-      </c>
-      <c r="DU1" t="str">
-        <v>assignTo_buffer_7</v>
-      </c>
-      <c r="DV1" t="str">
-        <v>assignTo_buffer_8</v>
-      </c>
-      <c r="DW1" t="str">
-        <v>assignTo_buffer_9</v>
-      </c>
-      <c r="DX1" t="str">
-        <v>assignTo_buffer_10</v>
-      </c>
-      <c r="DY1" t="str">
-        <v>assignTo_buffer_11</v>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
@@ -1107,78 +1035,6 @@
       <c r="DA2">
         <v>0</v>
       </c>
-      <c r="DB2">
-        <v>102</v>
-      </c>
-      <c r="DC2">
-        <v>152</v>
-      </c>
-      <c r="DD2">
-        <v>189</v>
-      </c>
-      <c r="DE2">
-        <v>80</v>
-      </c>
-      <c r="DF2">
-        <v>73</v>
-      </c>
-      <c r="DG2">
-        <v>9</v>
-      </c>
-      <c r="DH2">
-        <v>68</v>
-      </c>
-      <c r="DI2">
-        <v>85</v>
-      </c>
-      <c r="DJ2">
-        <v>53</v>
-      </c>
-      <c r="DK2">
-        <v>250</v>
-      </c>
-      <c r="DL2">
-        <v>106</v>
-      </c>
-      <c r="DM2">
-        <v>109</v>
-      </c>
-      <c r="DN2">
-        <v>102</v>
-      </c>
-      <c r="DO2">
-        <v>152</v>
-      </c>
-      <c r="DP2">
-        <v>192</v>
-      </c>
-      <c r="DQ2">
-        <v>219</v>
-      </c>
-      <c r="DR2">
-        <v>167</v>
-      </c>
-      <c r="DS2">
-        <v>9</v>
-      </c>
-      <c r="DT2">
-        <v>148</v>
-      </c>
-      <c r="DU2">
-        <v>134</v>
-      </c>
-      <c r="DV2">
-        <v>129</v>
-      </c>
-      <c r="DW2">
-        <v>46</v>
-      </c>
-      <c r="DX2">
-        <v>74</v>
-      </c>
-      <c r="DY2">
-        <v>19</v>
-      </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
@@ -1232,7 +1088,7 @@
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:DY3"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:DA3"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>